<commit_message>
Add some ICY planets images and data
</commit_message>
<xml_diff>
--- a/Details.xlsx
+++ b/Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Andrea\Code\EDDiscovery\HighResIcons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A41D407-6D00-42C9-9901-8B950955D51A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA2B783-0E1D-487B-801C-D94EAA7C61D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C47AFF1-0F2E-4E80-9439-97C38743854E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="105">
   <si>
     <t>Class</t>
   </si>
@@ -313,6 +313,39 @@
   </si>
   <si>
     <t>HMCv36</t>
+  </si>
+  <si>
+    <t>ICYv1</t>
+  </si>
+  <si>
+    <t>ICY</t>
+  </si>
+  <si>
+    <t>ICYv2</t>
+  </si>
+  <si>
+    <t>ICYv3</t>
+  </si>
+  <si>
+    <t>ICYv4</t>
+  </si>
+  <si>
+    <t>ICYv5</t>
+  </si>
+  <si>
+    <t>neon</t>
+  </si>
+  <si>
+    <t>ICYv6</t>
+  </si>
+  <si>
+    <t>nitrogen magma</t>
+  </si>
+  <si>
+    <t>ICYv7</t>
+  </si>
+  <si>
+    <t>ICYv8</t>
   </si>
 </sst>
 </file>
@@ -612,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -725,6 +758,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1040,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378DFCFD-A23B-459A-BDF7-1A47346AC4C8}">
-  <dimension ref="B1:W165"/>
+  <dimension ref="B1:X165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="V60" sqref="V60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,17 +1098,20 @@
     <col min="7" max="7" width="32.140625" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.7109375" style="26" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.7109375" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" ht="97.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:24" ht="97.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -1100,21 +1145,24 @@
       <c r="P1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="8"/>
       <c r="S1" s="8"/>
       <c r="T1" s="8"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="7" t="s">
+      <c r="U1" s="8"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="27" t="s">
         <v>5</v>
       </c>
@@ -1144,17 +1192,20 @@
       <c r="N2" s="35"/>
       <c r="O2" s="35"/>
       <c r="P2" s="35"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="31" t="s">
+      <c r="Q2" s="35"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="32"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="29" t="s">
+      <c r="T2" s="32"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="29" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="2:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+    </row>
+    <row r="3" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
       <c r="D3" s="3" t="s">
@@ -1172,19 +1223,22 @@
       <c r="N3" s="38"/>
       <c r="O3" s="38"/>
       <c r="P3" s="38"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="13" t="s">
+      <c r="Q3" s="38"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="U3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="30"/>
-    </row>
-    <row r="4" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V3" s="30"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+    </row>
+    <row r="4" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1214,19 +1268,22 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="9">
+      <c r="Q4" s="9"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="9">
         <v>65.5</v>
       </c>
-      <c r="S4" s="9">
+      <c r="T4" s="9">
         <v>34.5</v>
       </c>
-      <c r="T4" s="9"/>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="9"/>
+      <c r="V4" s="24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+    </row>
+    <row r="5" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1254,19 +1311,22 @@
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="9">
+      <c r="Q5" s="9"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="9">
         <v>67.099999999999994</v>
       </c>
-      <c r="S5" s="9">
+      <c r="T5" s="9">
         <v>32.9</v>
       </c>
-      <c r="T5" s="9"/>
-      <c r="U5" s="24" t="s">
+      <c r="U5" s="9"/>
+      <c r="V5" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+    </row>
+    <row r="6" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
@@ -1296,19 +1356,22 @@
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="9">
+      <c r="Q6" s="9"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="9">
         <v>67.2</v>
       </c>
-      <c r="S6" s="9">
+      <c r="T6" s="9">
         <v>32.799999999999997</v>
       </c>
-      <c r="T6" s="9"/>
-      <c r="U6" s="24" t="s">
+      <c r="U6" s="9"/>
+      <c r="V6" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+    </row>
+    <row r="7" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
@@ -1338,19 +1401,22 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="9">
+      <c r="Q7" s="9"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="9">
         <v>67.099999999999994</v>
       </c>
-      <c r="S7" s="9">
+      <c r="T7" s="9">
         <v>32.9</v>
       </c>
-      <c r="T7" s="9"/>
-      <c r="U7" s="24" t="s">
+      <c r="U7" s="9"/>
+      <c r="V7" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+    </row>
+    <row r="8" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1380,19 +1446,22 @@
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="9">
+      <c r="Q8" s="9"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="9">
         <v>67.099999999999994</v>
       </c>
-      <c r="S8" s="9">
+      <c r="T8" s="9">
         <v>32.9</v>
       </c>
-      <c r="T8" s="9"/>
-      <c r="U8" s="24" t="s">
+      <c r="U8" s="9"/>
+      <c r="V8" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+    </row>
+    <row r="9" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
@@ -1422,19 +1491,22 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="9">
+      <c r="Q9" s="9"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="9">
         <v>67.099999999999994</v>
       </c>
-      <c r="S9" s="9">
+      <c r="T9" s="9">
         <v>32.9</v>
       </c>
-      <c r="T9" s="9"/>
-      <c r="U9" s="24" t="s">
+      <c r="U9" s="9"/>
+      <c r="V9" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+    </row>
+    <row r="10" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1464,19 +1536,22 @@
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="9">
+      <c r="Q10" s="9"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="9">
         <v>67.099999999999994</v>
       </c>
-      <c r="S10" s="9">
+      <c r="T10" s="9">
         <v>32.9</v>
       </c>
-      <c r="T10" s="9"/>
-      <c r="U10" s="24" t="s">
+      <c r="U10" s="9"/>
+      <c r="V10" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+    </row>
+    <row r="11" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
@@ -1506,19 +1581,22 @@
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="9">
+      <c r="Q11" s="9"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="9">
         <v>66.5</v>
       </c>
-      <c r="S11" s="9">
+      <c r="T11" s="9">
         <v>33.5</v>
       </c>
-      <c r="T11" s="9"/>
-      <c r="U11" s="24" t="s">
+      <c r="U11" s="9"/>
+      <c r="V11" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+    </row>
+    <row r="12" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
@@ -1548,19 +1626,22 @@
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="9">
+      <c r="Q12" s="9"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="9">
         <v>66.5</v>
       </c>
-      <c r="S12" s="9">
+      <c r="T12" s="9">
         <v>33.5</v>
       </c>
-      <c r="T12" s="9"/>
-      <c r="U12" s="24" t="s">
+      <c r="U12" s="9"/>
+      <c r="V12" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+    </row>
+    <row r="13" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
@@ -1592,19 +1673,22 @@
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="9">
+      <c r="Q13" s="9"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="9">
         <v>68.2</v>
       </c>
-      <c r="S13" s="9">
+      <c r="T13" s="9">
         <v>31.8</v>
       </c>
-      <c r="T13" s="9"/>
-      <c r="U13" s="24" t="s">
+      <c r="U13" s="9"/>
+      <c r="V13" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+    </row>
+    <row r="14" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>29</v>
       </c>
@@ -1636,19 +1720,22 @@
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="9">
+      <c r="Q14" s="9"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="9">
         <v>66.900000000000006</v>
       </c>
-      <c r="S14" s="9">
+      <c r="T14" s="9">
         <v>33.1</v>
       </c>
-      <c r="T14" s="9"/>
-      <c r="U14" s="24" t="s">
+      <c r="U14" s="9"/>
+      <c r="V14" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+    </row>
+    <row r="15" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>30</v>
       </c>
@@ -1680,19 +1767,22 @@
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="9">
+      <c r="Q15" s="9"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="9">
         <v>65.900000000000006</v>
       </c>
-      <c r="S15" s="9">
+      <c r="T15" s="9">
         <v>34.1</v>
       </c>
-      <c r="T15" s="9"/>
-      <c r="U15" s="24" t="s">
+      <c r="U15" s="9"/>
+      <c r="V15" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+    </row>
+    <row r="16" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>44</v>
       </c>
@@ -1720,19 +1810,22 @@
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="9">
+      <c r="Q16" s="9"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="9">
         <v>67.2</v>
       </c>
-      <c r="S16" s="9">
+      <c r="T16" s="9">
         <v>32.799999999999997</v>
       </c>
-      <c r="T16" s="9"/>
-      <c r="U16" s="24" t="s">
+      <c r="U16" s="9"/>
+      <c r="V16" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+    </row>
+    <row r="17" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>49</v>
       </c>
@@ -1764,19 +1857,22 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="9">
+      <c r="Q17" s="9"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="9">
         <v>65.900000000000006</v>
       </c>
-      <c r="S17" s="9">
+      <c r="T17" s="9">
         <v>34.1</v>
       </c>
-      <c r="T17" s="9"/>
-      <c r="U17" s="24" t="s">
+      <c r="U17" s="9"/>
+      <c r="V17" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+    </row>
+    <row r="18" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>66</v>
       </c>
@@ -1794,7 +1890,7 @@
       <c r="H18" s="11">
         <v>0.2</v>
       </c>
-      <c r="I18" s="19"/>
+      <c r="I18" s="9"/>
       <c r="J18" s="9">
         <v>89.6</v>
       </c>
@@ -1806,19 +1902,22 @@
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="9">
+      <c r="Q18" s="9"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="9">
         <v>66.900000000000006</v>
       </c>
-      <c r="S18" s="9">
+      <c r="T18" s="9">
         <v>33.1</v>
       </c>
-      <c r="T18" s="9"/>
-      <c r="U18" s="24" t="s">
+      <c r="U18" s="9"/>
+      <c r="V18" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+    </row>
+    <row r="19" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>67</v>
       </c>
@@ -1836,7 +1935,7 @@
         <v>17</v>
       </c>
       <c r="H19" s="11"/>
-      <c r="I19" s="19"/>
+      <c r="I19" s="9"/>
       <c r="J19" s="9">
         <v>2.2000000000000002</v>
       </c>
@@ -1848,19 +1947,22 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="9"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="9">
+      <c r="Q19" s="9"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="9">
         <v>67.3</v>
       </c>
-      <c r="S19" s="9">
+      <c r="T19" s="9">
         <v>32.700000000000003</v>
       </c>
-      <c r="T19" s="9"/>
-      <c r="U19" s="24" t="s">
+      <c r="U19" s="9"/>
+      <c r="V19" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+    </row>
+    <row r="20" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>69</v>
       </c>
@@ -1878,7 +1980,7 @@
         <v>33</v>
       </c>
       <c r="H20" s="11"/>
-      <c r="I20" s="19"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="9">
         <v>97.2</v>
       </c>
@@ -1892,19 +1994,22 @@
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="9">
+      <c r="Q20" s="9"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="9">
         <v>67</v>
       </c>
-      <c r="S20" s="9">
+      <c r="T20" s="9">
         <v>33</v>
       </c>
-      <c r="T20" s="9"/>
-      <c r="U20" s="24" t="s">
+      <c r="U20" s="9"/>
+      <c r="V20" s="24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+    </row>
+    <row r="21" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>70</v>
       </c>
@@ -1936,19 +2041,22 @@
         <v>0.1</v>
       </c>
       <c r="P21" s="9"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="9">
+      <c r="Q21" s="9"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="9">
         <v>67.2</v>
       </c>
-      <c r="S21" s="9">
+      <c r="T21" s="9">
         <v>32.799999999999997</v>
       </c>
-      <c r="T21" s="9"/>
-      <c r="U21" s="24" t="s">
+      <c r="U21" s="9"/>
+      <c r="V21" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+    </row>
+    <row r="22" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>72</v>
       </c>
@@ -1966,7 +2074,7 @@
         <v>28</v>
       </c>
       <c r="H22" s="11"/>
-      <c r="I22" s="19"/>
+      <c r="I22" s="9"/>
       <c r="J22" s="9">
         <v>35</v>
       </c>
@@ -1980,19 +2088,22 @@
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="9">
+      <c r="Q22" s="9"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="9">
         <v>66.7</v>
       </c>
-      <c r="S22" s="9">
+      <c r="T22" s="9">
         <v>33.299999999999997</v>
       </c>
-      <c r="T22" s="9"/>
-      <c r="U22" s="24" t="s">
+      <c r="U22" s="9"/>
+      <c r="V22" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+    </row>
+    <row r="23" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>73</v>
       </c>
@@ -2010,7 +2121,7 @@
         <v>17</v>
       </c>
       <c r="H23" s="11"/>
-      <c r="I23" s="19"/>
+      <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9">
         <v>99.6</v>
@@ -2024,19 +2135,22 @@
       </c>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="9">
+      <c r="Q23" s="9"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="9">
         <v>67</v>
       </c>
-      <c r="S23" s="9">
+      <c r="T23" s="9">
         <v>33</v>
       </c>
-      <c r="T23" s="9"/>
-      <c r="U23" s="24" t="s">
+      <c r="U23" s="9"/>
+      <c r="V23" s="24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+    </row>
+    <row r="24" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>74</v>
       </c>
@@ -2054,7 +2168,7 @@
         <v>26</v>
       </c>
       <c r="H24" s="11"/>
-      <c r="I24" s="19"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="9">
         <v>33.1</v>
       </c>
@@ -2068,21 +2182,24 @@
       </c>
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="9">
+      <c r="Q24" s="9"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="9">
         <v>64.3</v>
       </c>
-      <c r="S24" s="9">
+      <c r="T24" s="9">
         <v>31.2</v>
       </c>
-      <c r="T24" s="9">
+      <c r="U24" s="9">
         <v>4.5</v>
       </c>
-      <c r="U24" s="24" t="s">
+      <c r="V24" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+    </row>
+    <row r="25" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>75</v>
       </c>
@@ -2102,7 +2219,7 @@
       <c r="H25" s="11">
         <v>0.3</v>
       </c>
-      <c r="I25" s="19"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="9">
         <v>99.7</v>
       </c>
@@ -2112,19 +2229,22 @@
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="9">
+      <c r="Q25" s="9"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="9">
         <v>66.900000000000006</v>
       </c>
-      <c r="S25" s="9">
+      <c r="T25" s="9">
         <v>33.1</v>
       </c>
-      <c r="T25" s="9"/>
-      <c r="U25" s="24" t="s">
+      <c r="U25" s="9"/>
+      <c r="V25" s="24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+    </row>
+    <row r="26" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>77</v>
       </c>
@@ -2152,19 +2272,22 @@
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="9">
+      <c r="Q26" s="9"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="9">
         <v>66.900000000000006</v>
       </c>
-      <c r="S26" s="9">
+      <c r="T26" s="9">
         <v>33.1</v>
       </c>
-      <c r="T26" s="9"/>
-      <c r="U26" s="24" t="s">
+      <c r="U26" s="9"/>
+      <c r="V26" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+    </row>
+    <row r="27" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
         <v>78</v>
       </c>
@@ -2194,19 +2317,22 @@
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="9">
+      <c r="Q27" s="9"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="9">
         <v>67.5</v>
       </c>
-      <c r="S27" s="9">
+      <c r="T27" s="9">
         <v>32.5</v>
       </c>
-      <c r="T27" s="9"/>
-      <c r="U27" s="24" t="s">
+      <c r="U27" s="9"/>
+      <c r="V27" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+    </row>
+    <row r="28" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>79</v>
       </c>
@@ -2236,19 +2362,22 @@
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="9">
+      <c r="Q28" s="9"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="9">
         <v>67.3</v>
       </c>
-      <c r="S28" s="9">
+      <c r="T28" s="9">
         <v>32.700000000000003</v>
       </c>
-      <c r="T28" s="9"/>
-      <c r="U28" s="24" t="s">
+      <c r="U28" s="9"/>
+      <c r="V28" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W28" s="8"/>
+      <c r="X28" s="8"/>
+    </row>
+    <row r="29" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>80</v>
       </c>
@@ -2278,21 +2407,24 @@
       <c r="P29" s="9">
         <v>0.6</v>
       </c>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="9">
+      <c r="Q29" s="9"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="9">
         <v>64</v>
       </c>
-      <c r="S29" s="9">
+      <c r="T29" s="9">
         <v>31.7</v>
       </c>
-      <c r="T29" s="9">
+      <c r="U29" s="9">
         <v>4.3</v>
       </c>
-      <c r="U29" s="24" t="s">
+      <c r="V29" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="30" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
+    </row>
+    <row r="30" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
         <v>82</v>
       </c>
@@ -2320,19 +2452,22 @@
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="9">
+      <c r="Q30" s="9"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="9">
         <v>67.099999999999994</v>
       </c>
-      <c r="S30" s="9">
+      <c r="T30" s="9">
         <v>32.9</v>
       </c>
-      <c r="T30" s="9"/>
-      <c r="U30" s="24" t="s">
+      <c r="U30" s="9"/>
+      <c r="V30" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="31" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
+    </row>
+    <row r="31" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
         <v>85</v>
       </c>
@@ -2362,19 +2497,22 @@
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="9">
+      <c r="Q31" s="9"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="9">
         <v>65.3</v>
       </c>
-      <c r="S31" s="9">
+      <c r="T31" s="9">
         <v>34.700000000000003</v>
       </c>
-      <c r="T31" s="9"/>
-      <c r="U31" s="24" t="s">
+      <c r="U31" s="9"/>
+      <c r="V31" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W31" s="8"/>
+      <c r="X31" s="8"/>
+    </row>
+    <row r="32" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
         <v>86</v>
       </c>
@@ -2387,23 +2525,37 @@
       <c r="E32" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="F32" s="8"/>
       <c r="G32" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="H32" s="41"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
       <c r="N32" s="5">
         <v>100</v>
       </c>
-      <c r="R32" s="9">
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="42"/>
+      <c r="S32" s="9">
         <v>67.3</v>
       </c>
-      <c r="S32" s="9">
+      <c r="T32" s="9">
         <v>32.700000000000003</v>
       </c>
-      <c r="U32" s="24" t="s">
+      <c r="U32" s="8"/>
+      <c r="V32" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="33" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
+    </row>
+    <row r="33" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
         <v>87</v>
       </c>
@@ -2429,19 +2581,22 @@
       <c r="N33" s="9"/>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="9">
+      <c r="Q33" s="9"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="9">
         <v>67.3</v>
       </c>
-      <c r="S33" s="9">
+      <c r="T33" s="9">
         <v>32.700000000000003</v>
       </c>
-      <c r="T33" s="9"/>
-      <c r="U33" s="24" t="s">
+      <c r="U33" s="9"/>
+      <c r="V33" s="24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W33" s="8"/>
+      <c r="X33" s="8"/>
+    </row>
+    <row r="34" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
         <v>88</v>
       </c>
@@ -2467,19 +2622,22 @@
       <c r="N34" s="9"/>
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="9">
+      <c r="Q34" s="9"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="9">
         <v>65.599999999999994</v>
       </c>
-      <c r="S34" s="9">
+      <c r="T34" s="9">
         <v>34.4</v>
       </c>
-      <c r="T34" s="9"/>
-      <c r="U34" s="24" t="s">
+      <c r="U34" s="9"/>
+      <c r="V34" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
+    </row>
+    <row r="35" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
         <v>89</v>
       </c>
@@ -2505,19 +2663,22 @@
       <c r="N35" s="9"/>
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="9">
+      <c r="Q35" s="9"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="9">
         <v>67</v>
       </c>
-      <c r="S35" s="9">
+      <c r="T35" s="9">
         <v>33</v>
       </c>
-      <c r="T35" s="9"/>
-      <c r="U35" s="24" t="s">
+      <c r="U35" s="9"/>
+      <c r="V35" s="24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="36" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W35" s="8"/>
+      <c r="X35" s="8"/>
+    </row>
+    <row r="36" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>90</v>
       </c>
@@ -2543,19 +2704,22 @@
       <c r="N36" s="9"/>
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="9">
+      <c r="Q36" s="9"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="9">
         <v>67.3</v>
       </c>
-      <c r="S36" s="9">
+      <c r="T36" s="9">
         <v>32.700000000000003</v>
       </c>
-      <c r="T36" s="9"/>
-      <c r="U36" s="24" t="s">
+      <c r="U36" s="9"/>
+      <c r="V36" s="24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="37" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W36" s="8"/>
+      <c r="X36" s="8"/>
+    </row>
+    <row r="37" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
         <v>91</v>
       </c>
@@ -2581,19 +2745,22 @@
       <c r="N37" s="9"/>
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="9">
+      <c r="Q37" s="9"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="9">
         <v>67</v>
       </c>
-      <c r="S37" s="9">
+      <c r="T37" s="9">
         <v>33</v>
       </c>
-      <c r="T37" s="9"/>
-      <c r="U37" s="24" t="s">
+      <c r="U37" s="9"/>
+      <c r="V37" s="24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="38" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W37" s="8"/>
+      <c r="X37" s="8"/>
+    </row>
+    <row r="38" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
         <v>92</v>
       </c>
@@ -2619,19 +2786,22 @@
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="9">
+      <c r="Q38" s="9"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="9">
         <v>67</v>
       </c>
-      <c r="S38" s="9">
+      <c r="T38" s="9">
         <v>33</v>
       </c>
-      <c r="T38" s="9"/>
-      <c r="U38" s="24" t="s">
+      <c r="U38" s="9"/>
+      <c r="V38" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W38" s="8"/>
+      <c r="X38" s="8"/>
+    </row>
+    <row r="39" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
         <v>93</v>
       </c>
@@ -2657,19 +2827,22 @@
       <c r="N39" s="9"/>
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
-      <c r="Q39" s="15"/>
-      <c r="R39" s="9">
+      <c r="Q39" s="9"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="9">
         <v>67.3</v>
       </c>
-      <c r="S39" s="9">
+      <c r="T39" s="9">
         <v>32.700000000000003</v>
       </c>
-      <c r="T39" s="9"/>
-      <c r="U39" s="24" t="s">
+      <c r="U39" s="9"/>
+      <c r="V39" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
+    </row>
+    <row r="40" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
         <v>52</v>
       </c>
@@ -2703,21 +2876,24 @@
       </c>
       <c r="O40" s="9"/>
       <c r="P40" s="9"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="9">
+      <c r="Q40" s="9"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="9">
         <v>66.7</v>
       </c>
-      <c r="S40" s="9">
+      <c r="T40" s="9">
         <v>32.799999999999997</v>
       </c>
-      <c r="T40" s="9">
+      <c r="U40" s="9">
         <v>1.5</v>
       </c>
-      <c r="U40" s="24" t="s">
+      <c r="V40" s="24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W40" s="8"/>
+      <c r="X40" s="8"/>
+    </row>
+    <row r="41" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
         <v>53</v>
       </c>
@@ -2751,19 +2927,22 @@
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
       <c r="P41" s="9"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="9">
+      <c r="Q41" s="9"/>
+      <c r="R41" s="15"/>
+      <c r="S41" s="9">
         <v>66.3</v>
       </c>
-      <c r="S41" s="9">
+      <c r="T41" s="9">
         <v>33.700000000000003</v>
       </c>
-      <c r="T41" s="9"/>
-      <c r="U41" s="24" t="s">
+      <c r="U41" s="9"/>
+      <c r="V41" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W41" s="8"/>
+      <c r="X41" s="8"/>
+    </row>
+    <row r="42" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
         <v>54</v>
       </c>
@@ -2797,19 +2976,22 @@
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="9">
+      <c r="Q42" s="9"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="9">
         <v>67.7</v>
       </c>
-      <c r="S42" s="9">
+      <c r="T42" s="9">
         <v>32.9</v>
       </c>
-      <c r="T42" s="9"/>
-      <c r="U42" s="24" t="s">
+      <c r="U42" s="9"/>
+      <c r="V42" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="43" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W42" s="8"/>
+      <c r="X42" s="8"/>
+    </row>
+    <row r="43" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
         <v>55</v>
       </c>
@@ -2843,19 +3025,22 @@
       </c>
       <c r="O43" s="9"/>
       <c r="P43" s="9"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="9">
+      <c r="Q43" s="9"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="9">
         <v>67.3</v>
       </c>
-      <c r="S43" s="9">
+      <c r="T43" s="9">
         <v>32.700000000000003</v>
       </c>
-      <c r="T43" s="9"/>
-      <c r="U43" s="24" t="s">
+      <c r="U43" s="9"/>
+      <c r="V43" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="44" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W43" s="8"/>
+      <c r="X43" s="8"/>
+    </row>
+    <row r="44" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
         <v>57</v>
       </c>
@@ -2889,19 +3074,22 @@
       <c r="N44" s="9"/>
       <c r="O44" s="9"/>
       <c r="P44" s="9"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="9">
+      <c r="Q44" s="9"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="9">
         <v>66.5</v>
       </c>
-      <c r="S44" s="9">
+      <c r="T44" s="9">
         <v>33.5</v>
       </c>
-      <c r="T44" s="9"/>
-      <c r="U44" s="24" t="s">
+      <c r="U44" s="9"/>
+      <c r="V44" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="45" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W44" s="8"/>
+      <c r="X44" s="8"/>
+    </row>
+    <row r="45" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
         <v>56</v>
       </c>
@@ -2935,21 +3123,24 @@
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
       <c r="P45" s="9"/>
-      <c r="Q45" s="15"/>
-      <c r="R45" s="9">
+      <c r="Q45" s="9"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="9">
         <v>66.2</v>
       </c>
-      <c r="S45" s="9">
+      <c r="T45" s="9">
         <v>32.9</v>
       </c>
-      <c r="T45" s="9">
+      <c r="U45" s="9">
         <v>0.9</v>
       </c>
-      <c r="U45" s="24" t="s">
+      <c r="V45" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="46" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W45" s="8"/>
+      <c r="X45" s="8"/>
+    </row>
+    <row r="46" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
         <v>59</v>
       </c>
@@ -2983,21 +3174,24 @@
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
       <c r="P46" s="9"/>
-      <c r="Q46" s="15"/>
-      <c r="R46" s="9">
+      <c r="Q46" s="9"/>
+      <c r="R46" s="15"/>
+      <c r="S46" s="9">
         <v>66.400000000000006</v>
       </c>
-      <c r="S46" s="9">
+      <c r="T46" s="9">
         <v>33.4</v>
       </c>
-      <c r="T46" s="9">
+      <c r="U46" s="9">
         <v>0.2</v>
       </c>
-      <c r="U46" s="24" t="s">
+      <c r="V46" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="47" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W46" s="8"/>
+      <c r="X46" s="8"/>
+    </row>
+    <row r="47" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
         <v>60</v>
       </c>
@@ -3031,19 +3225,22 @@
       <c r="N47" s="9"/>
       <c r="O47" s="9"/>
       <c r="P47" s="9"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="9">
+      <c r="Q47" s="9"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="9">
         <v>65.599999999999994</v>
       </c>
-      <c r="S47" s="9">
+      <c r="T47" s="9">
         <v>34.4</v>
       </c>
-      <c r="T47" s="9"/>
-      <c r="U47" s="24" t="s">
+      <c r="U47" s="9"/>
+      <c r="V47" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W47" s="8"/>
+      <c r="X47" s="8"/>
+    </row>
+    <row r="48" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B48" s="5" t="s">
         <v>34</v>
       </c>
@@ -3077,19 +3274,22 @@
       <c r="N48" s="9"/>
       <c r="O48" s="9"/>
       <c r="P48" s="9"/>
-      <c r="Q48" s="15"/>
-      <c r="R48" s="9">
+      <c r="Q48" s="9"/>
+      <c r="R48" s="15"/>
+      <c r="S48" s="9">
         <v>66.7</v>
       </c>
-      <c r="S48" s="9">
+      <c r="T48" s="9">
         <v>33.299999999999997</v>
       </c>
-      <c r="T48" s="9"/>
-      <c r="U48" s="24" t="s">
+      <c r="U48" s="9"/>
+      <c r="V48" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W48" s="8"/>
+      <c r="X48" s="8"/>
+    </row>
+    <row r="49" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
         <v>38</v>
       </c>
@@ -3123,19 +3323,22 @@
       <c r="N49" s="9"/>
       <c r="O49" s="9"/>
       <c r="P49" s="9"/>
-      <c r="Q49" s="15"/>
-      <c r="R49" s="9">
+      <c r="Q49" s="9"/>
+      <c r="R49" s="15"/>
+      <c r="S49" s="9">
         <v>67.099999999999994</v>
       </c>
-      <c r="S49" s="9">
+      <c r="T49" s="9">
         <v>32.9</v>
       </c>
-      <c r="T49" s="9"/>
-      <c r="U49" s="24" t="s">
+      <c r="U49" s="9"/>
+      <c r="V49" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W49" s="8"/>
+      <c r="X49" s="8"/>
+    </row>
+    <row r="50" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B50" s="5" t="s">
         <v>39</v>
       </c>
@@ -3167,19 +3370,22 @@
       <c r="N50" s="9"/>
       <c r="O50" s="9"/>
       <c r="P50" s="9"/>
-      <c r="Q50" s="15"/>
-      <c r="R50" s="9">
+      <c r="Q50" s="9"/>
+      <c r="R50" s="15"/>
+      <c r="S50" s="9">
         <v>67.099999999999994</v>
       </c>
-      <c r="S50" s="9">
+      <c r="T50" s="9">
         <v>32.9</v>
       </c>
-      <c r="T50" s="9"/>
-      <c r="U50" s="24" t="s">
+      <c r="U50" s="9"/>
+      <c r="V50" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W50" s="8"/>
+      <c r="X50" s="8"/>
+    </row>
+    <row r="51" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B51" s="5" t="s">
         <v>40</v>
       </c>
@@ -3211,199 +3417,386 @@
       <c r="P51" s="9">
         <v>9.1</v>
       </c>
-      <c r="Q51" s="15">
+      <c r="Q51" s="9"/>
+      <c r="R51" s="15">
         <v>0.1</v>
       </c>
-      <c r="R51" s="9">
+      <c r="S51" s="9">
         <v>21.1</v>
       </c>
-      <c r="S51" s="9">
+      <c r="T51" s="9">
         <v>10.3</v>
       </c>
-      <c r="T51" s="9">
+      <c r="U51" s="9">
         <v>68.599999999999994</v>
       </c>
-      <c r="U51" s="24" t="s">
+      <c r="V51" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
-      <c r="K52" s="19"/>
-      <c r="L52" s="19"/>
-      <c r="M52" s="19"/>
-      <c r="N52" s="19"/>
-      <c r="O52" s="19"/>
-      <c r="P52" s="19"/>
-      <c r="Q52" s="21"/>
-      <c r="R52" s="19"/>
-      <c r="S52" s="19"/>
-      <c r="T52" s="19"/>
-      <c r="U52" s="25"/>
-    </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
-      <c r="K53" s="19"/>
-      <c r="L53" s="19"/>
-      <c r="M53" s="19"/>
-      <c r="N53" s="19"/>
-      <c r="O53" s="19"/>
-      <c r="P53" s="19"/>
-      <c r="Q53" s="21"/>
-      <c r="R53" s="19"/>
-      <c r="S53" s="19"/>
-      <c r="T53" s="19"/>
-      <c r="U53" s="25"/>
-    </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="19"/>
-      <c r="J54" s="19"/>
-      <c r="K54" s="19"/>
-      <c r="L54" s="19"/>
-      <c r="M54" s="19"/>
-      <c r="N54" s="19"/>
-      <c r="O54" s="19"/>
-      <c r="P54" s="19"/>
-      <c r="Q54" s="21"/>
-      <c r="R54" s="19"/>
-      <c r="S54" s="19"/>
-      <c r="T54" s="19"/>
-      <c r="U54" s="25"/>
-    </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="19"/>
-      <c r="J55" s="19"/>
-      <c r="K55" s="19"/>
-      <c r="L55" s="19"/>
-      <c r="M55" s="19"/>
-      <c r="N55" s="19"/>
-      <c r="O55" s="19"/>
-      <c r="P55" s="19"/>
-      <c r="Q55" s="21"/>
-      <c r="R55" s="19"/>
-      <c r="S55" s="19"/>
-      <c r="T55" s="19"/>
-      <c r="U55" s="25"/>
-    </row>
-    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="20"/>
-      <c r="I56" s="19"/>
-      <c r="J56" s="19"/>
-      <c r="K56" s="19"/>
-      <c r="L56" s="19"/>
-      <c r="M56" s="19"/>
-      <c r="N56" s="19"/>
-      <c r="O56" s="19"/>
-      <c r="P56" s="19"/>
-      <c r="Q56" s="21"/>
-      <c r="R56" s="19"/>
-      <c r="S56" s="19"/>
-      <c r="T56" s="19"/>
-      <c r="U56" s="25"/>
-    </row>
-    <row r="57" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="20"/>
-      <c r="I57" s="19"/>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="19"/>
-      <c r="M57" s="19"/>
-      <c r="N57" s="19"/>
-      <c r="O57" s="19"/>
-      <c r="P57" s="19"/>
-      <c r="Q57" s="21"/>
-      <c r="R57" s="19"/>
-      <c r="S57" s="19"/>
-      <c r="T57" s="19"/>
-      <c r="U57" s="25"/>
-    </row>
-    <row r="58" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="19"/>
-      <c r="M58" s="19"/>
-      <c r="N58" s="19"/>
-      <c r="O58" s="19"/>
-      <c r="P58" s="19"/>
-      <c r="Q58" s="21"/>
-      <c r="R58" s="19"/>
-      <c r="S58" s="19"/>
-      <c r="T58" s="19"/>
-      <c r="U58" s="25"/>
-    </row>
-    <row r="59" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="19"/>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="19"/>
-      <c r="M59" s="19"/>
-      <c r="N59" s="19"/>
-      <c r="O59" s="19"/>
-      <c r="P59" s="19"/>
-      <c r="Q59" s="21"/>
-      <c r="R59" s="19"/>
-      <c r="S59" s="19"/>
-      <c r="T59" s="19"/>
-      <c r="U59" s="25"/>
-    </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W51" s="8"/>
+      <c r="X51" s="8"/>
+    </row>
+    <row r="52" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B52" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="5">
+        <v>93</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H52" s="11"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9">
+        <v>99.1</v>
+      </c>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
+      <c r="O52" s="9"/>
+      <c r="P52" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="Q52" s="9"/>
+      <c r="R52" s="15"/>
+      <c r="S52" s="9">
+        <v>21.3</v>
+      </c>
+      <c r="T52" s="9">
+        <v>10.4</v>
+      </c>
+      <c r="U52" s="9">
+        <v>68.3</v>
+      </c>
+      <c r="V52" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="W52" s="8"/>
+      <c r="X52" s="8"/>
+    </row>
+    <row r="53" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B53" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53" s="5">
+        <v>104</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53" s="11"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9">
+        <v>100</v>
+      </c>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="O53" s="9"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="9"/>
+      <c r="R53" s="15"/>
+      <c r="S53" s="9">
+        <v>21.3</v>
+      </c>
+      <c r="T53" s="9">
+        <v>10.6</v>
+      </c>
+      <c r="U53" s="9">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="V53" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="W53" s="8"/>
+      <c r="X53" s="8"/>
+    </row>
+    <row r="54" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B54" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D54" s="5">
+        <v>134</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" s="11"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9">
+        <v>99.9</v>
+      </c>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="N54" s="9"/>
+      <c r="O54" s="9"/>
+      <c r="P54" s="9"/>
+      <c r="Q54" s="9"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="9">
+        <v>32.4</v>
+      </c>
+      <c r="T54" s="9">
+        <v>15.5</v>
+      </c>
+      <c r="U54" s="9">
+        <v>52.1</v>
+      </c>
+      <c r="V54" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="W54" s="8"/>
+      <c r="X54" s="8"/>
+    </row>
+    <row r="55" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B55" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D55" s="5">
+        <v>151</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" s="11"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9">
+        <v>100</v>
+      </c>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="9"/>
+      <c r="P55" s="9"/>
+      <c r="Q55" s="9"/>
+      <c r="R55" s="15"/>
+      <c r="S55" s="9">
+        <v>21.2</v>
+      </c>
+      <c r="T55" s="9">
+        <v>10.4</v>
+      </c>
+      <c r="U55" s="9">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="V55" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="W55" s="8"/>
+      <c r="X55" s="8"/>
+    </row>
+    <row r="56" spans="2:24" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B56" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D56" s="5">
+        <v>108</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H56" s="11"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9">
+        <v>96</v>
+      </c>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="9">
+        <v>3.9</v>
+      </c>
+      <c r="Q56" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="R56" s="42"/>
+      <c r="S56" s="9">
+        <v>21.2</v>
+      </c>
+      <c r="T56" s="9">
+        <v>10.5</v>
+      </c>
+      <c r="U56" s="9">
+        <v>68.3</v>
+      </c>
+      <c r="V56" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="2:24" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B57" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" s="5">
+        <v>48</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H57" s="11"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9"/>
+      <c r="P57" s="9"/>
+      <c r="Q57" s="43">
+        <v>100</v>
+      </c>
+      <c r="R57" s="42"/>
+      <c r="S57" s="9">
+        <v>21.2</v>
+      </c>
+      <c r="T57" s="9">
+        <v>10.1</v>
+      </c>
+      <c r="U57" s="9">
+        <v>68.8</v>
+      </c>
+      <c r="V57" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="2:24" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B58" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D58" s="5">
+        <v>117</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H58" s="11"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
+      <c r="O58" s="9"/>
+      <c r="P58" s="9"/>
+      <c r="Q58" s="9"/>
+      <c r="R58" s="15"/>
+      <c r="S58" s="9">
+        <v>15.9</v>
+      </c>
+      <c r="T58" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="U58" s="9">
+        <v>82.5</v>
+      </c>
+      <c r="V58" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B59" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D59" s="5">
+        <v>128</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H59" s="11"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9">
+        <v>100</v>
+      </c>
+      <c r="N59" s="9"/>
+      <c r="O59" s="9"/>
+      <c r="P59" s="9"/>
+      <c r="Q59" s="9"/>
+      <c r="R59" s="15"/>
+      <c r="S59" s="9">
+        <v>21</v>
+      </c>
+      <c r="T59" s="9">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="U59" s="9">
+        <v>68.8</v>
+      </c>
+      <c r="V59" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="W59" s="8"/>
+      <c r="X59" s="8"/>
+    </row>
+    <row r="60" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -3419,13 +3812,14 @@
       <c r="N60" s="19"/>
       <c r="O60" s="19"/>
       <c r="P60" s="19"/>
-      <c r="Q60" s="21"/>
-      <c r="R60" s="19"/>
+      <c r="Q60" s="19"/>
+      <c r="R60" s="21"/>
       <c r="S60" s="19"/>
       <c r="T60" s="19"/>
-      <c r="U60" s="25"/>
-    </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U60" s="19"/>
+      <c r="V60" s="25"/>
+    </row>
+    <row r="61" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -3441,13 +3835,14 @@
       <c r="N61" s="19"/>
       <c r="O61" s="19"/>
       <c r="P61" s="19"/>
-      <c r="Q61" s="21"/>
-      <c r="R61" s="19"/>
+      <c r="Q61" s="19"/>
+      <c r="R61" s="21"/>
       <c r="S61" s="19"/>
       <c r="T61" s="19"/>
-      <c r="U61" s="25"/>
-    </row>
-    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U61" s="19"/>
+      <c r="V61" s="25"/>
+    </row>
+    <row r="62" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -3463,13 +3858,14 @@
       <c r="N62" s="19"/>
       <c r="O62" s="19"/>
       <c r="P62" s="19"/>
-      <c r="Q62" s="21"/>
-      <c r="R62" s="19"/>
+      <c r="Q62" s="19"/>
+      <c r="R62" s="21"/>
       <c r="S62" s="19"/>
       <c r="T62" s="19"/>
-      <c r="U62" s="25"/>
-    </row>
-    <row r="63" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U62" s="19"/>
+      <c r="V62" s="25"/>
+    </row>
+    <row r="63" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -3485,13 +3881,14 @@
       <c r="N63" s="19"/>
       <c r="O63" s="19"/>
       <c r="P63" s="19"/>
-      <c r="Q63" s="21"/>
-      <c r="R63" s="19"/>
+      <c r="Q63" s="19"/>
+      <c r="R63" s="21"/>
       <c r="S63" s="19"/>
       <c r="T63" s="19"/>
-      <c r="U63" s="25"/>
-    </row>
-    <row r="64" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U63" s="19"/>
+      <c r="V63" s="25"/>
+    </row>
+    <row r="64" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -3507,13 +3904,14 @@
       <c r="N64" s="19"/>
       <c r="O64" s="19"/>
       <c r="P64" s="19"/>
-      <c r="Q64" s="21"/>
-      <c r="R64" s="19"/>
+      <c r="Q64" s="19"/>
+      <c r="R64" s="21"/>
       <c r="S64" s="19"/>
       <c r="T64" s="19"/>
-      <c r="U64" s="25"/>
-    </row>
-    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U64" s="19"/>
+      <c r="V64" s="25"/>
+    </row>
+    <row r="65" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -3529,13 +3927,14 @@
       <c r="N65" s="19"/>
       <c r="O65" s="19"/>
       <c r="P65" s="19"/>
-      <c r="Q65" s="21"/>
-      <c r="R65" s="19"/>
+      <c r="Q65" s="19"/>
+      <c r="R65" s="21"/>
       <c r="S65" s="19"/>
       <c r="T65" s="19"/>
-      <c r="U65" s="25"/>
-    </row>
-    <row r="66" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U65" s="19"/>
+      <c r="V65" s="25"/>
+    </row>
+    <row r="66" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -3551,13 +3950,14 @@
       <c r="N66" s="19"/>
       <c r="O66" s="19"/>
       <c r="P66" s="19"/>
-      <c r="Q66" s="21"/>
-      <c r="R66" s="19"/>
+      <c r="Q66" s="19"/>
+      <c r="R66" s="21"/>
       <c r="S66" s="19"/>
       <c r="T66" s="19"/>
-      <c r="U66" s="25"/>
-    </row>
-    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U66" s="19"/>
+      <c r="V66" s="25"/>
+    </row>
+    <row r="67" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H67" s="20"/>
       <c r="I67" s="19"/>
       <c r="J67" s="19"/>
@@ -3567,12 +3967,13 @@
       <c r="N67" s="19"/>
       <c r="O67" s="19"/>
       <c r="P67" s="19"/>
-      <c r="Q67" s="21"/>
-      <c r="R67" s="22"/>
+      <c r="Q67" s="19"/>
+      <c r="R67" s="21"/>
       <c r="S67" s="22"/>
       <c r="T67" s="22"/>
-    </row>
-    <row r="68" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U67" s="22"/>
+    </row>
+    <row r="68" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H68" s="20"/>
       <c r="I68" s="19"/>
       <c r="J68" s="19"/>
@@ -3582,12 +3983,13 @@
       <c r="N68" s="19"/>
       <c r="O68" s="19"/>
       <c r="P68" s="19"/>
-      <c r="Q68" s="21"/>
-      <c r="R68" s="22"/>
+      <c r="Q68" s="19"/>
+      <c r="R68" s="21"/>
       <c r="S68" s="22"/>
       <c r="T68" s="22"/>
-    </row>
-    <row r="69" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U68" s="22"/>
+    </row>
+    <row r="69" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H69" s="20"/>
       <c r="I69" s="19"/>
       <c r="J69" s="19"/>
@@ -3597,12 +3999,13 @@
       <c r="N69" s="19"/>
       <c r="O69" s="19"/>
       <c r="P69" s="19"/>
-      <c r="Q69" s="21"/>
-      <c r="R69" s="22"/>
+      <c r="Q69" s="19"/>
+      <c r="R69" s="21"/>
       <c r="S69" s="22"/>
       <c r="T69" s="22"/>
-    </row>
-    <row r="70" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U69" s="22"/>
+    </row>
+    <row r="70" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H70" s="20"/>
       <c r="I70" s="19"/>
       <c r="J70" s="19"/>
@@ -3612,12 +4015,13 @@
       <c r="N70" s="19"/>
       <c r="O70" s="19"/>
       <c r="P70" s="19"/>
-      <c r="Q70" s="21"/>
-      <c r="R70" s="22"/>
+      <c r="Q70" s="19"/>
+      <c r="R70" s="21"/>
       <c r="S70" s="22"/>
       <c r="T70" s="22"/>
-    </row>
-    <row r="71" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U70" s="22"/>
+    </row>
+    <row r="71" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H71" s="20"/>
       <c r="I71" s="19"/>
       <c r="J71" s="19"/>
@@ -3627,12 +4031,13 @@
       <c r="N71" s="19"/>
       <c r="O71" s="19"/>
       <c r="P71" s="19"/>
-      <c r="Q71" s="21"/>
-      <c r="R71" s="22"/>
+      <c r="Q71" s="19"/>
+      <c r="R71" s="21"/>
       <c r="S71" s="22"/>
       <c r="T71" s="22"/>
-    </row>
-    <row r="72" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U71" s="22"/>
+    </row>
+    <row r="72" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H72" s="20"/>
       <c r="I72" s="19"/>
       <c r="J72" s="19"/>
@@ -3642,12 +4047,13 @@
       <c r="N72" s="19"/>
       <c r="O72" s="19"/>
       <c r="P72" s="19"/>
-      <c r="Q72" s="21"/>
-      <c r="R72" s="22"/>
+      <c r="Q72" s="19"/>
+      <c r="R72" s="21"/>
       <c r="S72" s="22"/>
       <c r="T72" s="22"/>
-    </row>
-    <row r="73" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U72" s="22"/>
+    </row>
+    <row r="73" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H73" s="20"/>
       <c r="I73" s="19"/>
       <c r="J73" s="19"/>
@@ -3657,12 +4063,13 @@
       <c r="N73" s="19"/>
       <c r="O73" s="19"/>
       <c r="P73" s="19"/>
-      <c r="Q73" s="21"/>
-      <c r="R73" s="22"/>
+      <c r="Q73" s="19"/>
+      <c r="R73" s="21"/>
       <c r="S73" s="22"/>
       <c r="T73" s="22"/>
-    </row>
-    <row r="74" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U73" s="22"/>
+    </row>
+    <row r="74" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H74" s="20"/>
       <c r="I74" s="19"/>
       <c r="J74" s="19"/>
@@ -3672,12 +4079,13 @@
       <c r="N74" s="19"/>
       <c r="O74" s="19"/>
       <c r="P74" s="19"/>
-      <c r="Q74" s="21"/>
-      <c r="R74" s="22"/>
+      <c r="Q74" s="19"/>
+      <c r="R74" s="21"/>
       <c r="S74" s="22"/>
       <c r="T74" s="22"/>
-    </row>
-    <row r="75" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U74" s="22"/>
+    </row>
+    <row r="75" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H75" s="20"/>
       <c r="I75" s="19"/>
       <c r="J75" s="19"/>
@@ -3687,12 +4095,13 @@
       <c r="N75" s="19"/>
       <c r="O75" s="19"/>
       <c r="P75" s="19"/>
-      <c r="Q75" s="21"/>
-      <c r="R75" s="22"/>
+      <c r="Q75" s="19"/>
+      <c r="R75" s="21"/>
       <c r="S75" s="22"/>
       <c r="T75" s="22"/>
-    </row>
-    <row r="76" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U75" s="22"/>
+    </row>
+    <row r="76" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H76" s="20"/>
       <c r="I76" s="19"/>
       <c r="J76" s="19"/>
@@ -3702,12 +4111,13 @@
       <c r="N76" s="19"/>
       <c r="O76" s="19"/>
       <c r="P76" s="19"/>
-      <c r="Q76" s="21"/>
-      <c r="R76" s="22"/>
+      <c r="Q76" s="19"/>
+      <c r="R76" s="21"/>
       <c r="S76" s="22"/>
       <c r="T76" s="22"/>
-    </row>
-    <row r="77" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U76" s="22"/>
+    </row>
+    <row r="77" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H77" s="20"/>
       <c r="I77" s="19"/>
       <c r="J77" s="19"/>
@@ -3717,12 +4127,13 @@
       <c r="N77" s="19"/>
       <c r="O77" s="19"/>
       <c r="P77" s="19"/>
-      <c r="Q77" s="21"/>
-      <c r="R77" s="22"/>
+      <c r="Q77" s="19"/>
+      <c r="R77" s="21"/>
       <c r="S77" s="22"/>
       <c r="T77" s="22"/>
-    </row>
-    <row r="78" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U77" s="22"/>
+    </row>
+    <row r="78" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H78" s="20"/>
       <c r="I78" s="19"/>
       <c r="J78" s="19"/>
@@ -3732,12 +4143,13 @@
       <c r="N78" s="19"/>
       <c r="O78" s="19"/>
       <c r="P78" s="19"/>
-      <c r="Q78" s="21"/>
-      <c r="R78" s="22"/>
+      <c r="Q78" s="19"/>
+      <c r="R78" s="21"/>
       <c r="S78" s="22"/>
       <c r="T78" s="22"/>
-    </row>
-    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U78" s="22"/>
+    </row>
+    <row r="79" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H79" s="20"/>
       <c r="I79" s="19"/>
       <c r="J79" s="19"/>
@@ -3747,12 +4159,13 @@
       <c r="N79" s="19"/>
       <c r="O79" s="19"/>
       <c r="P79" s="19"/>
-      <c r="Q79" s="21"/>
-      <c r="R79" s="22"/>
+      <c r="Q79" s="19"/>
+      <c r="R79" s="21"/>
       <c r="S79" s="22"/>
       <c r="T79" s="22"/>
-    </row>
-    <row r="80" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U79" s="22"/>
+    </row>
+    <row r="80" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H80" s="20"/>
       <c r="I80" s="19"/>
       <c r="J80" s="19"/>
@@ -3762,12 +4175,13 @@
       <c r="N80" s="19"/>
       <c r="O80" s="19"/>
       <c r="P80" s="19"/>
-      <c r="Q80" s="21"/>
-      <c r="R80" s="22"/>
+      <c r="Q80" s="19"/>
+      <c r="R80" s="21"/>
       <c r="S80" s="22"/>
       <c r="T80" s="22"/>
-    </row>
-    <row r="81" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U80" s="22"/>
+    </row>
+    <row r="81" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H81" s="20"/>
       <c r="I81" s="19"/>
       <c r="J81" s="19"/>
@@ -3777,12 +4191,13 @@
       <c r="N81" s="19"/>
       <c r="O81" s="19"/>
       <c r="P81" s="19"/>
-      <c r="Q81" s="21"/>
-      <c r="R81" s="22"/>
+      <c r="Q81" s="19"/>
+      <c r="R81" s="21"/>
       <c r="S81" s="22"/>
       <c r="T81" s="22"/>
-    </row>
-    <row r="82" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U81" s="22"/>
+    </row>
+    <row r="82" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H82" s="20"/>
       <c r="I82" s="19"/>
       <c r="J82" s="19"/>
@@ -3792,12 +4207,13 @@
       <c r="N82" s="19"/>
       <c r="O82" s="19"/>
       <c r="P82" s="19"/>
-      <c r="Q82" s="21"/>
-      <c r="R82" s="22"/>
+      <c r="Q82" s="19"/>
+      <c r="R82" s="21"/>
       <c r="S82" s="22"/>
       <c r="T82" s="22"/>
-    </row>
-    <row r="83" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U82" s="22"/>
+    </row>
+    <row r="83" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H83" s="20"/>
       <c r="I83" s="19"/>
       <c r="J83" s="19"/>
@@ -3807,12 +4223,13 @@
       <c r="N83" s="19"/>
       <c r="O83" s="19"/>
       <c r="P83" s="19"/>
-      <c r="Q83" s="21"/>
-      <c r="R83" s="22"/>
+      <c r="Q83" s="19"/>
+      <c r="R83" s="21"/>
       <c r="S83" s="22"/>
       <c r="T83" s="22"/>
-    </row>
-    <row r="84" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U83" s="22"/>
+    </row>
+    <row r="84" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H84" s="20"/>
       <c r="I84" s="19"/>
       <c r="J84" s="19"/>
@@ -3822,12 +4239,13 @@
       <c r="N84" s="19"/>
       <c r="O84" s="19"/>
       <c r="P84" s="19"/>
-      <c r="Q84" s="21"/>
-      <c r="R84" s="22"/>
+      <c r="Q84" s="19"/>
+      <c r="R84" s="21"/>
       <c r="S84" s="22"/>
       <c r="T84" s="22"/>
-    </row>
-    <row r="85" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U84" s="22"/>
+    </row>
+    <row r="85" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H85" s="20"/>
       <c r="I85" s="19"/>
       <c r="J85" s="19"/>
@@ -3837,12 +4255,13 @@
       <c r="N85" s="19"/>
       <c r="O85" s="19"/>
       <c r="P85" s="19"/>
-      <c r="Q85" s="21"/>
-      <c r="R85" s="22"/>
+      <c r="Q85" s="19"/>
+      <c r="R85" s="21"/>
       <c r="S85" s="22"/>
       <c r="T85" s="22"/>
-    </row>
-    <row r="86" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U85" s="22"/>
+    </row>
+    <row r="86" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H86" s="20"/>
       <c r="I86" s="19"/>
       <c r="J86" s="19"/>
@@ -3852,12 +4271,13 @@
       <c r="N86" s="19"/>
       <c r="O86" s="19"/>
       <c r="P86" s="19"/>
-      <c r="Q86" s="21"/>
-      <c r="R86" s="22"/>
+      <c r="Q86" s="19"/>
+      <c r="R86" s="21"/>
       <c r="S86" s="22"/>
       <c r="T86" s="22"/>
-    </row>
-    <row r="87" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U86" s="22"/>
+    </row>
+    <row r="87" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H87" s="20"/>
       <c r="I87" s="19"/>
       <c r="J87" s="19"/>
@@ -3867,12 +4287,13 @@
       <c r="N87" s="19"/>
       <c r="O87" s="19"/>
       <c r="P87" s="19"/>
-      <c r="Q87" s="21"/>
-      <c r="R87" s="22"/>
+      <c r="Q87" s="19"/>
+      <c r="R87" s="21"/>
       <c r="S87" s="22"/>
       <c r="T87" s="22"/>
-    </row>
-    <row r="88" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U87" s="22"/>
+    </row>
+    <row r="88" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H88" s="20"/>
       <c r="I88" s="19"/>
       <c r="J88" s="19"/>
@@ -3882,12 +4303,13 @@
       <c r="N88" s="19"/>
       <c r="O88" s="19"/>
       <c r="P88" s="19"/>
-      <c r="Q88" s="21"/>
-      <c r="R88" s="22"/>
+      <c r="Q88" s="19"/>
+      <c r="R88" s="21"/>
       <c r="S88" s="22"/>
       <c r="T88" s="22"/>
-    </row>
-    <row r="89" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U88" s="22"/>
+    </row>
+    <row r="89" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H89" s="20"/>
       <c r="I89" s="19"/>
       <c r="J89" s="19"/>
@@ -3897,12 +4319,13 @@
       <c r="N89" s="19"/>
       <c r="O89" s="19"/>
       <c r="P89" s="19"/>
-      <c r="Q89" s="21"/>
-      <c r="R89" s="22"/>
+      <c r="Q89" s="19"/>
+      <c r="R89" s="21"/>
       <c r="S89" s="22"/>
       <c r="T89" s="22"/>
-    </row>
-    <row r="90" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U89" s="22"/>
+    </row>
+    <row r="90" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H90" s="20"/>
       <c r="I90" s="19"/>
       <c r="J90" s="19"/>
@@ -3912,12 +4335,13 @@
       <c r="N90" s="19"/>
       <c r="O90" s="19"/>
       <c r="P90" s="19"/>
-      <c r="Q90" s="21"/>
-      <c r="R90" s="22"/>
+      <c r="Q90" s="19"/>
+      <c r="R90" s="21"/>
       <c r="S90" s="22"/>
       <c r="T90" s="22"/>
-    </row>
-    <row r="91" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U90" s="22"/>
+    </row>
+    <row r="91" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H91" s="20"/>
       <c r="I91" s="19"/>
       <c r="J91" s="19"/>
@@ -3927,12 +4351,13 @@
       <c r="N91" s="19"/>
       <c r="O91" s="19"/>
       <c r="P91" s="19"/>
-      <c r="Q91" s="21"/>
-      <c r="R91" s="22"/>
+      <c r="Q91" s="19"/>
+      <c r="R91" s="21"/>
       <c r="S91" s="22"/>
       <c r="T91" s="22"/>
-    </row>
-    <row r="92" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U91" s="22"/>
+    </row>
+    <row r="92" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H92" s="20"/>
       <c r="I92" s="19"/>
       <c r="J92" s="19"/>
@@ -3942,12 +4367,13 @@
       <c r="N92" s="19"/>
       <c r="O92" s="19"/>
       <c r="P92" s="19"/>
-      <c r="Q92" s="21"/>
-      <c r="R92" s="22"/>
+      <c r="Q92" s="19"/>
+      <c r="R92" s="21"/>
       <c r="S92" s="22"/>
       <c r="T92" s="22"/>
-    </row>
-    <row r="93" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U92" s="22"/>
+    </row>
+    <row r="93" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H93" s="20"/>
       <c r="I93" s="19"/>
       <c r="J93" s="19"/>
@@ -3957,12 +4383,13 @@
       <c r="N93" s="19"/>
       <c r="O93" s="19"/>
       <c r="P93" s="19"/>
-      <c r="Q93" s="21"/>
-      <c r="R93" s="22"/>
+      <c r="Q93" s="19"/>
+      <c r="R93" s="21"/>
       <c r="S93" s="22"/>
       <c r="T93" s="22"/>
-    </row>
-    <row r="94" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U93" s="22"/>
+    </row>
+    <row r="94" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H94" s="20"/>
       <c r="I94" s="19"/>
       <c r="J94" s="19"/>
@@ -3972,12 +4399,13 @@
       <c r="N94" s="19"/>
       <c r="O94" s="19"/>
       <c r="P94" s="19"/>
-      <c r="Q94" s="21"/>
-      <c r="R94" s="22"/>
+      <c r="Q94" s="19"/>
+      <c r="R94" s="21"/>
       <c r="S94" s="22"/>
       <c r="T94" s="22"/>
-    </row>
-    <row r="95" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U94" s="22"/>
+    </row>
+    <row r="95" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H95" s="20"/>
       <c r="I95" s="19"/>
       <c r="J95" s="19"/>
@@ -3987,12 +4415,13 @@
       <c r="N95" s="19"/>
       <c r="O95" s="19"/>
       <c r="P95" s="19"/>
-      <c r="Q95" s="21"/>
-      <c r="R95" s="22"/>
+      <c r="Q95" s="19"/>
+      <c r="R95" s="21"/>
       <c r="S95" s="22"/>
       <c r="T95" s="22"/>
-    </row>
-    <row r="96" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U95" s="22"/>
+    </row>
+    <row r="96" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H96" s="20"/>
       <c r="I96" s="19"/>
       <c r="J96" s="19"/>
@@ -4002,12 +4431,13 @@
       <c r="N96" s="19"/>
       <c r="O96" s="19"/>
       <c r="P96" s="19"/>
-      <c r="Q96" s="21"/>
-      <c r="R96" s="22"/>
+      <c r="Q96" s="19"/>
+      <c r="R96" s="21"/>
       <c r="S96" s="22"/>
       <c r="T96" s="22"/>
-    </row>
-    <row r="97" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U96" s="22"/>
+    </row>
+    <row r="97" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H97" s="20"/>
       <c r="I97" s="19"/>
       <c r="J97" s="19"/>
@@ -4017,12 +4447,13 @@
       <c r="N97" s="19"/>
       <c r="O97" s="19"/>
       <c r="P97" s="19"/>
-      <c r="Q97" s="21"/>
-      <c r="R97" s="22"/>
+      <c r="Q97" s="19"/>
+      <c r="R97" s="21"/>
       <c r="S97" s="22"/>
       <c r="T97" s="22"/>
-    </row>
-    <row r="98" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U97" s="22"/>
+    </row>
+    <row r="98" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H98" s="20"/>
       <c r="I98" s="19"/>
       <c r="J98" s="19"/>
@@ -4032,12 +4463,13 @@
       <c r="N98" s="19"/>
       <c r="O98" s="19"/>
       <c r="P98" s="19"/>
-      <c r="Q98" s="21"/>
-      <c r="R98" s="22"/>
+      <c r="Q98" s="19"/>
+      <c r="R98" s="21"/>
       <c r="S98" s="22"/>
       <c r="T98" s="22"/>
-    </row>
-    <row r="99" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U98" s="22"/>
+    </row>
+    <row r="99" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H99" s="20"/>
       <c r="I99" s="19"/>
       <c r="J99" s="19"/>
@@ -4047,12 +4479,13 @@
       <c r="N99" s="19"/>
       <c r="O99" s="19"/>
       <c r="P99" s="19"/>
-      <c r="Q99" s="21"/>
-      <c r="R99" s="22"/>
+      <c r="Q99" s="19"/>
+      <c r="R99" s="21"/>
       <c r="S99" s="22"/>
       <c r="T99" s="22"/>
-    </row>
-    <row r="100" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U99" s="22"/>
+    </row>
+    <row r="100" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H100" s="20"/>
       <c r="I100" s="19"/>
       <c r="J100" s="19"/>
@@ -4062,12 +4495,13 @@
       <c r="N100" s="19"/>
       <c r="O100" s="19"/>
       <c r="P100" s="19"/>
-      <c r="Q100" s="21"/>
-      <c r="R100" s="22"/>
+      <c r="Q100" s="19"/>
+      <c r="R100" s="21"/>
       <c r="S100" s="22"/>
       <c r="T100" s="22"/>
-    </row>
-    <row r="101" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U100" s="22"/>
+    </row>
+    <row r="101" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H101" s="20"/>
       <c r="I101" s="19"/>
       <c r="J101" s="19"/>
@@ -4077,12 +4511,13 @@
       <c r="N101" s="19"/>
       <c r="O101" s="19"/>
       <c r="P101" s="19"/>
-      <c r="Q101" s="21"/>
-      <c r="R101" s="22"/>
+      <c r="Q101" s="19"/>
+      <c r="R101" s="21"/>
       <c r="S101" s="22"/>
       <c r="T101" s="22"/>
-    </row>
-    <row r="102" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U101" s="22"/>
+    </row>
+    <row r="102" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H102" s="20"/>
       <c r="I102" s="19"/>
       <c r="J102" s="19"/>
@@ -4092,12 +4527,13 @@
       <c r="N102" s="19"/>
       <c r="O102" s="19"/>
       <c r="P102" s="19"/>
-      <c r="Q102" s="21"/>
-      <c r="R102" s="22"/>
+      <c r="Q102" s="19"/>
+      <c r="R102" s="21"/>
       <c r="S102" s="22"/>
       <c r="T102" s="22"/>
-    </row>
-    <row r="103" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U102" s="22"/>
+    </row>
+    <row r="103" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H103" s="20"/>
       <c r="I103" s="19"/>
       <c r="J103" s="19"/>
@@ -4107,12 +4543,13 @@
       <c r="N103" s="19"/>
       <c r="O103" s="19"/>
       <c r="P103" s="19"/>
-      <c r="Q103" s="21"/>
-      <c r="R103" s="22"/>
+      <c r="Q103" s="19"/>
+      <c r="R103" s="21"/>
       <c r="S103" s="22"/>
       <c r="T103" s="22"/>
-    </row>
-    <row r="104" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U103" s="22"/>
+    </row>
+    <row r="104" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H104" s="20"/>
       <c r="I104" s="19"/>
       <c r="J104" s="19"/>
@@ -4122,12 +4559,13 @@
       <c r="N104" s="19"/>
       <c r="O104" s="19"/>
       <c r="P104" s="19"/>
-      <c r="Q104" s="21"/>
-      <c r="R104" s="22"/>
+      <c r="Q104" s="19"/>
+      <c r="R104" s="21"/>
       <c r="S104" s="22"/>
       <c r="T104" s="22"/>
-    </row>
-    <row r="105" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U104" s="22"/>
+    </row>
+    <row r="105" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H105" s="20"/>
       <c r="I105" s="19"/>
       <c r="J105" s="19"/>
@@ -4137,12 +4575,13 @@
       <c r="N105" s="19"/>
       <c r="O105" s="19"/>
       <c r="P105" s="19"/>
-      <c r="Q105" s="21"/>
-      <c r="R105" s="22"/>
+      <c r="Q105" s="19"/>
+      <c r="R105" s="21"/>
       <c r="S105" s="22"/>
       <c r="T105" s="22"/>
-    </row>
-    <row r="106" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U105" s="22"/>
+    </row>
+    <row r="106" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H106" s="20"/>
       <c r="I106" s="19"/>
       <c r="J106" s="19"/>
@@ -4152,12 +4591,13 @@
       <c r="N106" s="19"/>
       <c r="O106" s="19"/>
       <c r="P106" s="19"/>
-      <c r="Q106" s="21"/>
-      <c r="R106" s="22"/>
+      <c r="Q106" s="19"/>
+      <c r="R106" s="21"/>
       <c r="S106" s="22"/>
       <c r="T106" s="22"/>
-    </row>
-    <row r="107" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U106" s="22"/>
+    </row>
+    <row r="107" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H107" s="20"/>
       <c r="I107" s="19"/>
       <c r="J107" s="19"/>
@@ -4167,12 +4607,13 @@
       <c r="N107" s="19"/>
       <c r="O107" s="19"/>
       <c r="P107" s="19"/>
-      <c r="Q107" s="21"/>
-      <c r="R107" s="22"/>
+      <c r="Q107" s="19"/>
+      <c r="R107" s="21"/>
       <c r="S107" s="22"/>
       <c r="T107" s="22"/>
-    </row>
-    <row r="108" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U107" s="22"/>
+    </row>
+    <row r="108" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H108" s="20"/>
       <c r="I108" s="19"/>
       <c r="J108" s="19"/>
@@ -4182,12 +4623,13 @@
       <c r="N108" s="19"/>
       <c r="O108" s="19"/>
       <c r="P108" s="19"/>
-      <c r="Q108" s="21"/>
-      <c r="R108" s="22"/>
+      <c r="Q108" s="19"/>
+      <c r="R108" s="21"/>
       <c r="S108" s="22"/>
       <c r="T108" s="22"/>
-    </row>
-    <row r="109" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U108" s="22"/>
+    </row>
+    <row r="109" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H109" s="20"/>
       <c r="I109" s="19"/>
       <c r="J109" s="19"/>
@@ -4197,12 +4639,13 @@
       <c r="N109" s="19"/>
       <c r="O109" s="19"/>
       <c r="P109" s="19"/>
-      <c r="Q109" s="21"/>
-      <c r="R109" s="22"/>
+      <c r="Q109" s="19"/>
+      <c r="R109" s="21"/>
       <c r="S109" s="22"/>
       <c r="T109" s="22"/>
-    </row>
-    <row r="110" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U109" s="22"/>
+    </row>
+    <row r="110" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H110" s="20"/>
       <c r="I110" s="19"/>
       <c r="J110" s="19"/>
@@ -4212,12 +4655,13 @@
       <c r="N110" s="19"/>
       <c r="O110" s="19"/>
       <c r="P110" s="19"/>
-      <c r="Q110" s="21"/>
-      <c r="R110" s="22"/>
+      <c r="Q110" s="19"/>
+      <c r="R110" s="21"/>
       <c r="S110" s="22"/>
       <c r="T110" s="22"/>
-    </row>
-    <row r="111" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U110" s="22"/>
+    </row>
+    <row r="111" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H111" s="20"/>
       <c r="I111" s="19"/>
       <c r="J111" s="19"/>
@@ -4227,12 +4671,13 @@
       <c r="N111" s="19"/>
       <c r="O111" s="19"/>
       <c r="P111" s="19"/>
-      <c r="Q111" s="21"/>
-      <c r="R111" s="22"/>
+      <c r="Q111" s="19"/>
+      <c r="R111" s="21"/>
       <c r="S111" s="22"/>
       <c r="T111" s="22"/>
-    </row>
-    <row r="112" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U111" s="22"/>
+    </row>
+    <row r="112" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H112" s="20"/>
       <c r="I112" s="19"/>
       <c r="J112" s="19"/>
@@ -4242,12 +4687,13 @@
       <c r="N112" s="19"/>
       <c r="O112" s="19"/>
       <c r="P112" s="19"/>
-      <c r="Q112" s="21"/>
-      <c r="R112" s="22"/>
+      <c r="Q112" s="19"/>
+      <c r="R112" s="21"/>
       <c r="S112" s="22"/>
       <c r="T112" s="22"/>
-    </row>
-    <row r="113" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U112" s="22"/>
+    </row>
+    <row r="113" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H113" s="20"/>
       <c r="I113" s="19"/>
       <c r="J113" s="19"/>
@@ -4257,12 +4703,13 @@
       <c r="N113" s="19"/>
       <c r="O113" s="19"/>
       <c r="P113" s="19"/>
-      <c r="Q113" s="21"/>
-      <c r="R113" s="22"/>
+      <c r="Q113" s="19"/>
+      <c r="R113" s="21"/>
       <c r="S113" s="22"/>
       <c r="T113" s="22"/>
-    </row>
-    <row r="114" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U113" s="22"/>
+    </row>
+    <row r="114" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H114" s="20"/>
       <c r="I114" s="19"/>
       <c r="J114" s="19"/>
@@ -4272,12 +4719,13 @@
       <c r="N114" s="19"/>
       <c r="O114" s="19"/>
       <c r="P114" s="19"/>
-      <c r="Q114" s="21"/>
-      <c r="R114" s="22"/>
+      <c r="Q114" s="19"/>
+      <c r="R114" s="21"/>
       <c r="S114" s="22"/>
       <c r="T114" s="22"/>
-    </row>
-    <row r="115" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U114" s="22"/>
+    </row>
+    <row r="115" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H115" s="20"/>
       <c r="I115" s="19"/>
       <c r="J115" s="19"/>
@@ -4287,12 +4735,13 @@
       <c r="N115" s="19"/>
       <c r="O115" s="19"/>
       <c r="P115" s="19"/>
-      <c r="Q115" s="21"/>
-      <c r="R115" s="22"/>
+      <c r="Q115" s="19"/>
+      <c r="R115" s="21"/>
       <c r="S115" s="22"/>
       <c r="T115" s="22"/>
-    </row>
-    <row r="116" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U115" s="22"/>
+    </row>
+    <row r="116" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H116" s="20"/>
       <c r="I116" s="19"/>
       <c r="J116" s="19"/>
@@ -4302,12 +4751,13 @@
       <c r="N116" s="19"/>
       <c r="O116" s="19"/>
       <c r="P116" s="19"/>
-      <c r="Q116" s="21"/>
-      <c r="R116" s="22"/>
+      <c r="Q116" s="19"/>
+      <c r="R116" s="21"/>
       <c r="S116" s="22"/>
       <c r="T116" s="22"/>
-    </row>
-    <row r="117" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U116" s="22"/>
+    </row>
+    <row r="117" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H117" s="20"/>
       <c r="I117" s="19"/>
       <c r="J117" s="19"/>
@@ -4317,12 +4767,13 @@
       <c r="N117" s="19"/>
       <c r="O117" s="19"/>
       <c r="P117" s="19"/>
-      <c r="Q117" s="21"/>
-      <c r="R117" s="22"/>
+      <c r="Q117" s="19"/>
+      <c r="R117" s="21"/>
       <c r="S117" s="22"/>
       <c r="T117" s="22"/>
-    </row>
-    <row r="118" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U117" s="22"/>
+    </row>
+    <row r="118" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H118" s="20"/>
       <c r="I118" s="19"/>
       <c r="J118" s="19"/>
@@ -4332,12 +4783,13 @@
       <c r="N118" s="19"/>
       <c r="O118" s="19"/>
       <c r="P118" s="19"/>
-      <c r="Q118" s="21"/>
-      <c r="R118" s="22"/>
+      <c r="Q118" s="19"/>
+      <c r="R118" s="21"/>
       <c r="S118" s="22"/>
       <c r="T118" s="22"/>
-    </row>
-    <row r="119" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U118" s="22"/>
+    </row>
+    <row r="119" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H119" s="20"/>
       <c r="I119" s="19"/>
       <c r="J119" s="19"/>
@@ -4347,12 +4799,13 @@
       <c r="N119" s="19"/>
       <c r="O119" s="19"/>
       <c r="P119" s="19"/>
-      <c r="Q119" s="21"/>
-      <c r="R119" s="22"/>
+      <c r="Q119" s="19"/>
+      <c r="R119" s="21"/>
       <c r="S119" s="22"/>
       <c r="T119" s="22"/>
-    </row>
-    <row r="120" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U119" s="22"/>
+    </row>
+    <row r="120" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H120" s="20"/>
       <c r="I120" s="19"/>
       <c r="J120" s="19"/>
@@ -4362,12 +4815,13 @@
       <c r="N120" s="19"/>
       <c r="O120" s="19"/>
       <c r="P120" s="19"/>
-      <c r="Q120" s="21"/>
-      <c r="R120" s="22"/>
+      <c r="Q120" s="19"/>
+      <c r="R120" s="21"/>
       <c r="S120" s="22"/>
       <c r="T120" s="22"/>
-    </row>
-    <row r="121" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U120" s="22"/>
+    </row>
+    <row r="121" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H121" s="20"/>
       <c r="I121" s="19"/>
       <c r="J121" s="19"/>
@@ -4377,12 +4831,13 @@
       <c r="N121" s="19"/>
       <c r="O121" s="19"/>
       <c r="P121" s="19"/>
-      <c r="Q121" s="21"/>
-      <c r="R121" s="22"/>
+      <c r="Q121" s="19"/>
+      <c r="R121" s="21"/>
       <c r="S121" s="22"/>
       <c r="T121" s="22"/>
-    </row>
-    <row r="122" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U121" s="22"/>
+    </row>
+    <row r="122" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H122" s="20"/>
       <c r="I122" s="19"/>
       <c r="J122" s="19"/>
@@ -4392,12 +4847,13 @@
       <c r="N122" s="19"/>
       <c r="O122" s="19"/>
       <c r="P122" s="19"/>
-      <c r="Q122" s="21"/>
-      <c r="R122" s="22"/>
+      <c r="Q122" s="19"/>
+      <c r="R122" s="21"/>
       <c r="S122" s="22"/>
       <c r="T122" s="22"/>
-    </row>
-    <row r="123" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U122" s="22"/>
+    </row>
+    <row r="123" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H123" s="20"/>
       <c r="I123" s="19"/>
       <c r="J123" s="19"/>
@@ -4407,12 +4863,13 @@
       <c r="N123" s="19"/>
       <c r="O123" s="19"/>
       <c r="P123" s="19"/>
-      <c r="Q123" s="21"/>
-      <c r="R123" s="22"/>
+      <c r="Q123" s="19"/>
+      <c r="R123" s="21"/>
       <c r="S123" s="22"/>
       <c r="T123" s="22"/>
-    </row>
-    <row r="124" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U123" s="22"/>
+    </row>
+    <row r="124" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H124" s="20"/>
       <c r="I124" s="19"/>
       <c r="J124" s="19"/>
@@ -4422,12 +4879,13 @@
       <c r="N124" s="19"/>
       <c r="O124" s="19"/>
       <c r="P124" s="19"/>
-      <c r="Q124" s="21"/>
-      <c r="R124" s="22"/>
+      <c r="Q124" s="19"/>
+      <c r="R124" s="21"/>
       <c r="S124" s="22"/>
       <c r="T124" s="22"/>
-    </row>
-    <row r="125" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U124" s="22"/>
+    </row>
+    <row r="125" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H125" s="20"/>
       <c r="I125" s="19"/>
       <c r="J125" s="19"/>
@@ -4437,12 +4895,13 @@
       <c r="N125" s="19"/>
       <c r="O125" s="19"/>
       <c r="P125" s="19"/>
-      <c r="Q125" s="21"/>
-      <c r="R125" s="22"/>
+      <c r="Q125" s="19"/>
+      <c r="R125" s="21"/>
       <c r="S125" s="22"/>
       <c r="T125" s="22"/>
-    </row>
-    <row r="126" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U125" s="22"/>
+    </row>
+    <row r="126" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H126" s="20"/>
       <c r="I126" s="19"/>
       <c r="J126" s="19"/>
@@ -4452,12 +4911,13 @@
       <c r="N126" s="19"/>
       <c r="O126" s="19"/>
       <c r="P126" s="19"/>
-      <c r="Q126" s="21"/>
-      <c r="R126" s="22"/>
+      <c r="Q126" s="19"/>
+      <c r="R126" s="21"/>
       <c r="S126" s="22"/>
       <c r="T126" s="22"/>
-    </row>
-    <row r="127" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U126" s="22"/>
+    </row>
+    <row r="127" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H127" s="20"/>
       <c r="I127" s="19"/>
       <c r="J127" s="19"/>
@@ -4467,12 +4927,13 @@
       <c r="N127" s="19"/>
       <c r="O127" s="19"/>
       <c r="P127" s="19"/>
-      <c r="Q127" s="21"/>
-      <c r="R127" s="22"/>
+      <c r="Q127" s="19"/>
+      <c r="R127" s="21"/>
       <c r="S127" s="22"/>
       <c r="T127" s="22"/>
-    </row>
-    <row r="128" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U127" s="22"/>
+    </row>
+    <row r="128" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H128" s="20"/>
       <c r="I128" s="19"/>
       <c r="J128" s="19"/>
@@ -4482,12 +4943,13 @@
       <c r="N128" s="19"/>
       <c r="O128" s="19"/>
       <c r="P128" s="19"/>
-      <c r="Q128" s="21"/>
-      <c r="R128" s="22"/>
+      <c r="Q128" s="19"/>
+      <c r="R128" s="21"/>
       <c r="S128" s="22"/>
       <c r="T128" s="22"/>
-    </row>
-    <row r="129" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U128" s="22"/>
+    </row>
+    <row r="129" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H129" s="20"/>
       <c r="I129" s="19"/>
       <c r="J129" s="19"/>
@@ -4497,12 +4959,13 @@
       <c r="N129" s="19"/>
       <c r="O129" s="19"/>
       <c r="P129" s="19"/>
-      <c r="Q129" s="21"/>
-      <c r="R129" s="22"/>
+      <c r="Q129" s="19"/>
+      <c r="R129" s="21"/>
       <c r="S129" s="22"/>
       <c r="T129" s="22"/>
-    </row>
-    <row r="130" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U129" s="22"/>
+    </row>
+    <row r="130" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H130" s="20"/>
       <c r="I130" s="19"/>
       <c r="J130" s="19"/>
@@ -4512,12 +4975,13 @@
       <c r="N130" s="19"/>
       <c r="O130" s="19"/>
       <c r="P130" s="19"/>
-      <c r="Q130" s="21"/>
-      <c r="R130" s="22"/>
+      <c r="Q130" s="19"/>
+      <c r="R130" s="21"/>
       <c r="S130" s="22"/>
       <c r="T130" s="22"/>
-    </row>
-    <row r="131" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U130" s="22"/>
+    </row>
+    <row r="131" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H131" s="20"/>
       <c r="I131" s="19"/>
       <c r="J131" s="19"/>
@@ -4527,12 +4991,13 @@
       <c r="N131" s="19"/>
       <c r="O131" s="19"/>
       <c r="P131" s="19"/>
-      <c r="Q131" s="21"/>
-      <c r="R131" s="22"/>
+      <c r="Q131" s="19"/>
+      <c r="R131" s="21"/>
       <c r="S131" s="22"/>
       <c r="T131" s="22"/>
-    </row>
-    <row r="132" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U131" s="22"/>
+    </row>
+    <row r="132" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H132" s="20"/>
       <c r="I132" s="19"/>
       <c r="J132" s="19"/>
@@ -4542,12 +5007,13 @@
       <c r="N132" s="19"/>
       <c r="O132" s="19"/>
       <c r="P132" s="19"/>
-      <c r="Q132" s="21"/>
-      <c r="R132" s="22"/>
+      <c r="Q132" s="19"/>
+      <c r="R132" s="21"/>
       <c r="S132" s="22"/>
       <c r="T132" s="22"/>
-    </row>
-    <row r="133" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U132" s="22"/>
+    </row>
+    <row r="133" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H133" s="20"/>
       <c r="I133" s="19"/>
       <c r="J133" s="19"/>
@@ -4557,12 +5023,13 @@
       <c r="N133" s="19"/>
       <c r="O133" s="19"/>
       <c r="P133" s="19"/>
-      <c r="Q133" s="21"/>
-      <c r="R133" s="22"/>
+      <c r="Q133" s="19"/>
+      <c r="R133" s="21"/>
       <c r="S133" s="22"/>
       <c r="T133" s="22"/>
-    </row>
-    <row r="134" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U133" s="22"/>
+    </row>
+    <row r="134" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H134" s="20"/>
       <c r="I134" s="19"/>
       <c r="J134" s="19"/>
@@ -4572,12 +5039,13 @@
       <c r="N134" s="19"/>
       <c r="O134" s="19"/>
       <c r="P134" s="19"/>
-      <c r="Q134" s="21"/>
-      <c r="R134" s="22"/>
+      <c r="Q134" s="19"/>
+      <c r="R134" s="21"/>
       <c r="S134" s="22"/>
       <c r="T134" s="22"/>
-    </row>
-    <row r="135" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U134" s="22"/>
+    </row>
+    <row r="135" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H135" s="20"/>
       <c r="I135" s="19"/>
       <c r="J135" s="19"/>
@@ -4587,12 +5055,13 @@
       <c r="N135" s="19"/>
       <c r="O135" s="19"/>
       <c r="P135" s="19"/>
-      <c r="Q135" s="21"/>
-      <c r="R135" s="22"/>
+      <c r="Q135" s="19"/>
+      <c r="R135" s="21"/>
       <c r="S135" s="22"/>
       <c r="T135" s="22"/>
-    </row>
-    <row r="136" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U135" s="22"/>
+    </row>
+    <row r="136" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H136" s="20"/>
       <c r="I136" s="19"/>
       <c r="J136" s="19"/>
@@ -4602,12 +5071,13 @@
       <c r="N136" s="19"/>
       <c r="O136" s="19"/>
       <c r="P136" s="19"/>
-      <c r="Q136" s="21"/>
-      <c r="R136" s="22"/>
+      <c r="Q136" s="19"/>
+      <c r="R136" s="21"/>
       <c r="S136" s="22"/>
       <c r="T136" s="22"/>
-    </row>
-    <row r="137" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U136" s="22"/>
+    </row>
+    <row r="137" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H137" s="20"/>
       <c r="I137" s="19"/>
       <c r="J137" s="19"/>
@@ -4617,12 +5087,13 @@
       <c r="N137" s="19"/>
       <c r="O137" s="19"/>
       <c r="P137" s="19"/>
-      <c r="Q137" s="21"/>
-      <c r="R137" s="22"/>
+      <c r="Q137" s="19"/>
+      <c r="R137" s="21"/>
       <c r="S137" s="22"/>
       <c r="T137" s="22"/>
-    </row>
-    <row r="138" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U137" s="22"/>
+    </row>
+    <row r="138" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H138" s="20"/>
       <c r="I138" s="19"/>
       <c r="J138" s="19"/>
@@ -4632,12 +5103,13 @@
       <c r="N138" s="19"/>
       <c r="O138" s="19"/>
       <c r="P138" s="19"/>
-      <c r="Q138" s="21"/>
-      <c r="R138" s="22"/>
+      <c r="Q138" s="19"/>
+      <c r="R138" s="21"/>
       <c r="S138" s="22"/>
       <c r="T138" s="22"/>
-    </row>
-    <row r="139" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U138" s="22"/>
+    </row>
+    <row r="139" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H139" s="20"/>
       <c r="I139" s="19"/>
       <c r="J139" s="19"/>
@@ -4647,12 +5119,13 @@
       <c r="N139" s="19"/>
       <c r="O139" s="19"/>
       <c r="P139" s="19"/>
-      <c r="Q139" s="21"/>
-      <c r="R139" s="22"/>
+      <c r="Q139" s="19"/>
+      <c r="R139" s="21"/>
       <c r="S139" s="22"/>
       <c r="T139" s="22"/>
-    </row>
-    <row r="140" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U139" s="22"/>
+    </row>
+    <row r="140" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H140" s="20"/>
       <c r="I140" s="19"/>
       <c r="J140" s="19"/>
@@ -4662,12 +5135,13 @@
       <c r="N140" s="19"/>
       <c r="O140" s="19"/>
       <c r="P140" s="19"/>
-      <c r="Q140" s="21"/>
-      <c r="R140" s="22"/>
+      <c r="Q140" s="19"/>
+      <c r="R140" s="21"/>
       <c r="S140" s="22"/>
       <c r="T140" s="22"/>
-    </row>
-    <row r="141" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U140" s="22"/>
+    </row>
+    <row r="141" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H141" s="20"/>
       <c r="I141" s="19"/>
       <c r="J141" s="19"/>
@@ -4677,12 +5151,13 @@
       <c r="N141" s="19"/>
       <c r="O141" s="19"/>
       <c r="P141" s="19"/>
-      <c r="Q141" s="21"/>
-      <c r="R141" s="22"/>
+      <c r="Q141" s="19"/>
+      <c r="R141" s="21"/>
       <c r="S141" s="22"/>
       <c r="T141" s="22"/>
-    </row>
-    <row r="142" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U141" s="22"/>
+    </row>
+    <row r="142" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H142" s="20"/>
       <c r="I142" s="19"/>
       <c r="J142" s="19"/>
@@ -4692,12 +5167,13 @@
       <c r="N142" s="19"/>
       <c r="O142" s="19"/>
       <c r="P142" s="19"/>
-      <c r="Q142" s="21"/>
-      <c r="R142" s="22"/>
+      <c r="Q142" s="19"/>
+      <c r="R142" s="21"/>
       <c r="S142" s="22"/>
       <c r="T142" s="22"/>
-    </row>
-    <row r="143" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U142" s="22"/>
+    </row>
+    <row r="143" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H143" s="20"/>
       <c r="I143" s="19"/>
       <c r="J143" s="19"/>
@@ -4707,12 +5183,13 @@
       <c r="N143" s="19"/>
       <c r="O143" s="19"/>
       <c r="P143" s="19"/>
-      <c r="Q143" s="21"/>
-      <c r="R143" s="22"/>
+      <c r="Q143" s="19"/>
+      <c r="R143" s="21"/>
       <c r="S143" s="22"/>
       <c r="T143" s="22"/>
-    </row>
-    <row r="144" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U143" s="22"/>
+    </row>
+    <row r="144" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H144" s="20"/>
       <c r="I144" s="19"/>
       <c r="J144" s="19"/>
@@ -4722,12 +5199,13 @@
       <c r="N144" s="19"/>
       <c r="O144" s="19"/>
       <c r="P144" s="19"/>
-      <c r="Q144" s="21"/>
-      <c r="R144" s="22"/>
+      <c r="Q144" s="19"/>
+      <c r="R144" s="21"/>
       <c r="S144" s="22"/>
       <c r="T144" s="22"/>
-    </row>
-    <row r="145" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U144" s="22"/>
+    </row>
+    <row r="145" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H145" s="20"/>
       <c r="I145" s="19"/>
       <c r="J145" s="19"/>
@@ -4737,12 +5215,13 @@
       <c r="N145" s="19"/>
       <c r="O145" s="19"/>
       <c r="P145" s="19"/>
-      <c r="Q145" s="21"/>
-      <c r="R145" s="22"/>
+      <c r="Q145" s="19"/>
+      <c r="R145" s="21"/>
       <c r="S145" s="22"/>
       <c r="T145" s="22"/>
-    </row>
-    <row r="146" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U145" s="22"/>
+    </row>
+    <row r="146" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H146" s="20"/>
       <c r="I146" s="19"/>
       <c r="J146" s="19"/>
@@ -4752,12 +5231,13 @@
       <c r="N146" s="19"/>
       <c r="O146" s="19"/>
       <c r="P146" s="19"/>
-      <c r="Q146" s="21"/>
-      <c r="R146" s="22"/>
+      <c r="Q146" s="19"/>
+      <c r="R146" s="21"/>
       <c r="S146" s="22"/>
       <c r="T146" s="22"/>
-    </row>
-    <row r="147" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U146" s="22"/>
+    </row>
+    <row r="147" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H147" s="20"/>
       <c r="I147" s="19"/>
       <c r="J147" s="19"/>
@@ -4767,12 +5247,13 @@
       <c r="N147" s="19"/>
       <c r="O147" s="19"/>
       <c r="P147" s="19"/>
-      <c r="Q147" s="21"/>
-      <c r="R147" s="22"/>
+      <c r="Q147" s="19"/>
+      <c r="R147" s="21"/>
       <c r="S147" s="22"/>
       <c r="T147" s="22"/>
-    </row>
-    <row r="148" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U147" s="22"/>
+    </row>
+    <row r="148" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H148" s="20"/>
       <c r="I148" s="19"/>
       <c r="J148" s="19"/>
@@ -4782,12 +5263,13 @@
       <c r="N148" s="19"/>
       <c r="O148" s="19"/>
       <c r="P148" s="19"/>
-      <c r="Q148" s="21"/>
-      <c r="R148" s="22"/>
+      <c r="Q148" s="19"/>
+      <c r="R148" s="21"/>
       <c r="S148" s="22"/>
       <c r="T148" s="22"/>
-    </row>
-    <row r="149" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U148" s="22"/>
+    </row>
+    <row r="149" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H149" s="20"/>
       <c r="I149" s="19"/>
       <c r="J149" s="19"/>
@@ -4797,12 +5279,13 @@
       <c r="N149" s="19"/>
       <c r="O149" s="19"/>
       <c r="P149" s="19"/>
-      <c r="Q149" s="21"/>
-      <c r="R149" s="22"/>
+      <c r="Q149" s="19"/>
+      <c r="R149" s="21"/>
       <c r="S149" s="22"/>
       <c r="T149" s="22"/>
-    </row>
-    <row r="150" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U149" s="22"/>
+    </row>
+    <row r="150" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H150" s="20"/>
       <c r="I150" s="19"/>
       <c r="J150" s="19"/>
@@ -4812,12 +5295,13 @@
       <c r="N150" s="19"/>
       <c r="O150" s="19"/>
       <c r="P150" s="19"/>
-      <c r="Q150" s="21"/>
-      <c r="R150" s="22"/>
+      <c r="Q150" s="19"/>
+      <c r="R150" s="21"/>
       <c r="S150" s="22"/>
       <c r="T150" s="22"/>
-    </row>
-    <row r="151" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U150" s="22"/>
+    </row>
+    <row r="151" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H151" s="20"/>
       <c r="I151" s="19"/>
       <c r="J151" s="19"/>
@@ -4827,12 +5311,13 @@
       <c r="N151" s="19"/>
       <c r="O151" s="19"/>
       <c r="P151" s="19"/>
-      <c r="Q151" s="21"/>
-      <c r="R151" s="22"/>
+      <c r="Q151" s="19"/>
+      <c r="R151" s="21"/>
       <c r="S151" s="22"/>
       <c r="T151" s="22"/>
-    </row>
-    <row r="152" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U151" s="22"/>
+    </row>
+    <row r="152" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H152" s="20"/>
       <c r="I152" s="19"/>
       <c r="J152" s="19"/>
@@ -4842,12 +5327,13 @@
       <c r="N152" s="19"/>
       <c r="O152" s="19"/>
       <c r="P152" s="19"/>
-      <c r="Q152" s="21"/>
-      <c r="R152" s="22"/>
+      <c r="Q152" s="19"/>
+      <c r="R152" s="21"/>
       <c r="S152" s="22"/>
       <c r="T152" s="22"/>
-    </row>
-    <row r="153" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U152" s="22"/>
+    </row>
+    <row r="153" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H153" s="20"/>
       <c r="I153" s="19"/>
       <c r="J153" s="19"/>
@@ -4857,12 +5343,13 @@
       <c r="N153" s="19"/>
       <c r="O153" s="19"/>
       <c r="P153" s="19"/>
-      <c r="Q153" s="21"/>
-      <c r="R153" s="22"/>
+      <c r="Q153" s="19"/>
+      <c r="R153" s="21"/>
       <c r="S153" s="22"/>
       <c r="T153" s="22"/>
-    </row>
-    <row r="154" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U153" s="22"/>
+    </row>
+    <row r="154" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H154" s="20"/>
       <c r="I154" s="19"/>
       <c r="J154" s="19"/>
@@ -4872,12 +5359,13 @@
       <c r="N154" s="19"/>
       <c r="O154" s="19"/>
       <c r="P154" s="19"/>
-      <c r="Q154" s="21"/>
-      <c r="R154" s="22"/>
+      <c r="Q154" s="19"/>
+      <c r="R154" s="21"/>
       <c r="S154" s="22"/>
       <c r="T154" s="22"/>
-    </row>
-    <row r="155" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U154" s="22"/>
+    </row>
+    <row r="155" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H155" s="20"/>
       <c r="I155" s="19"/>
       <c r="J155" s="19"/>
@@ -4887,12 +5375,13 @@
       <c r="N155" s="19"/>
       <c r="O155" s="19"/>
       <c r="P155" s="19"/>
-      <c r="Q155" s="21"/>
-      <c r="R155" s="22"/>
+      <c r="Q155" s="19"/>
+      <c r="R155" s="21"/>
       <c r="S155" s="22"/>
       <c r="T155" s="22"/>
-    </row>
-    <row r="156" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U155" s="22"/>
+    </row>
+    <row r="156" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H156" s="20"/>
       <c r="I156" s="19"/>
       <c r="J156" s="19"/>
@@ -4902,12 +5391,13 @@
       <c r="N156" s="19"/>
       <c r="O156" s="19"/>
       <c r="P156" s="19"/>
-      <c r="Q156" s="21"/>
-      <c r="R156" s="22"/>
+      <c r="Q156" s="19"/>
+      <c r="R156" s="21"/>
       <c r="S156" s="22"/>
       <c r="T156" s="22"/>
-    </row>
-    <row r="157" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U156" s="22"/>
+    </row>
+    <row r="157" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H157" s="20"/>
       <c r="I157" s="19"/>
       <c r="J157" s="19"/>
@@ -4917,12 +5407,13 @@
       <c r="N157" s="19"/>
       <c r="O157" s="19"/>
       <c r="P157" s="19"/>
-      <c r="Q157" s="21"/>
-      <c r="R157" s="22"/>
+      <c r="Q157" s="19"/>
+      <c r="R157" s="21"/>
       <c r="S157" s="22"/>
       <c r="T157" s="22"/>
-    </row>
-    <row r="158" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U157" s="22"/>
+    </row>
+    <row r="158" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H158" s="20"/>
       <c r="I158" s="19"/>
       <c r="J158" s="19"/>
@@ -4932,12 +5423,13 @@
       <c r="N158" s="19"/>
       <c r="O158" s="19"/>
       <c r="P158" s="19"/>
-      <c r="Q158" s="21"/>
-      <c r="R158" s="22"/>
+      <c r="Q158" s="19"/>
+      <c r="R158" s="21"/>
       <c r="S158" s="22"/>
       <c r="T158" s="22"/>
-    </row>
-    <row r="159" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U158" s="22"/>
+    </row>
+    <row r="159" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H159" s="20"/>
       <c r="I159" s="19"/>
       <c r="J159" s="19"/>
@@ -4947,12 +5439,13 @@
       <c r="N159" s="19"/>
       <c r="O159" s="19"/>
       <c r="P159" s="19"/>
-      <c r="Q159" s="21"/>
-      <c r="R159" s="22"/>
+      <c r="Q159" s="19"/>
+      <c r="R159" s="21"/>
       <c r="S159" s="22"/>
       <c r="T159" s="22"/>
-    </row>
-    <row r="160" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U159" s="22"/>
+    </row>
+    <row r="160" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H160" s="20"/>
       <c r="I160" s="19"/>
       <c r="J160" s="19"/>
@@ -4962,12 +5455,13 @@
       <c r="N160" s="19"/>
       <c r="O160" s="19"/>
       <c r="P160" s="19"/>
-      <c r="Q160" s="21"/>
-      <c r="R160" s="22"/>
+      <c r="Q160" s="19"/>
+      <c r="R160" s="21"/>
       <c r="S160" s="22"/>
       <c r="T160" s="22"/>
-    </row>
-    <row r="161" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U160" s="22"/>
+    </row>
+    <row r="161" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H161" s="20"/>
       <c r="I161" s="19"/>
       <c r="J161" s="19"/>
@@ -4977,12 +5471,13 @@
       <c r="N161" s="19"/>
       <c r="O161" s="19"/>
       <c r="P161" s="19"/>
-      <c r="Q161" s="21"/>
-      <c r="R161" s="22"/>
+      <c r="Q161" s="19"/>
+      <c r="R161" s="21"/>
       <c r="S161" s="22"/>
       <c r="T161" s="22"/>
-    </row>
-    <row r="162" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U161" s="22"/>
+    </row>
+    <row r="162" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H162" s="20"/>
       <c r="I162" s="19"/>
       <c r="J162" s="19"/>
@@ -4992,12 +5487,13 @@
       <c r="N162" s="19"/>
       <c r="O162" s="19"/>
       <c r="P162" s="19"/>
-      <c r="Q162" s="21"/>
-      <c r="R162" s="22"/>
+      <c r="Q162" s="19"/>
+      <c r="R162" s="21"/>
       <c r="S162" s="22"/>
       <c r="T162" s="22"/>
-    </row>
-    <row r="163" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U162" s="22"/>
+    </row>
+    <row r="163" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H163" s="20"/>
       <c r="I163" s="19"/>
       <c r="J163" s="19"/>
@@ -5007,12 +5503,13 @@
       <c r="N163" s="19"/>
       <c r="O163" s="19"/>
       <c r="P163" s="19"/>
-      <c r="Q163" s="21"/>
-      <c r="R163" s="22"/>
+      <c r="Q163" s="19"/>
+      <c r="R163" s="21"/>
       <c r="S163" s="22"/>
       <c r="T163" s="22"/>
-    </row>
-    <row r="164" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U163" s="22"/>
+    </row>
+    <row r="164" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H164" s="20"/>
       <c r="I164" s="19"/>
       <c r="J164" s="19"/>
@@ -5022,12 +5519,13 @@
       <c r="N164" s="19"/>
       <c r="O164" s="19"/>
       <c r="P164" s="19"/>
-      <c r="Q164" s="21"/>
-      <c r="R164" s="22"/>
+      <c r="Q164" s="19"/>
+      <c r="R164" s="21"/>
       <c r="S164" s="22"/>
       <c r="T164" s="22"/>
-    </row>
-    <row r="165" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="U164" s="22"/>
+    </row>
+    <row r="165" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H165" s="20"/>
       <c r="I165" s="19"/>
       <c r="J165" s="19"/>
@@ -5037,19 +5535,20 @@
       <c r="N165" s="19"/>
       <c r="O165" s="19"/>
       <c r="P165" s="19"/>
-      <c r="Q165" s="21"/>
-      <c r="R165" s="22"/>
+      <c r="Q165" s="19"/>
+      <c r="R165" s="21"/>
       <c r="S165" s="22"/>
       <c r="T165" s="22"/>
+      <c r="U165" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="H2:Q3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="H2:R3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="F2:F3"/>
   </mergeCells>

</xml_diff>